<commit_message>
ok 15 points optimisés, rapport à boucler
</commit_message>
<xml_diff>
--- a/audit/Modèle-audit-SEO.xlsx
+++ b/audit/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Documents\PROJET4\audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C45CD38-42B2-4BF2-A62D-707415403583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA73E02-B06D-45D4-B7FE-A01CF7FD3FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>Catégorie</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Aucun effet au survol sur la barre de navigation</t>
-  </si>
-  <si>
-    <t>Balises &lt;alt&gt; mal renseignées</t>
   </si>
   <si>
     <t>Créer une rubrique actualité</t>
@@ -472,14 +469,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -487,17 +487,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -716,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1004"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -781,316 +778,312 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>61</v>
+      <c r="E5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" spans="1:26" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="D9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:26" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="1:26" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="21"/>
-    </row>
-    <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="F17" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:26" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="22" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="23"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1101,13 +1094,12 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
@@ -1124,42 +1116,36 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E25" s="2"/>
-    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2115,20 +2101,19 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="F17:F18"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
16e point optimisé : contact amélioré
</commit_message>
<xml_diff>
--- a/audit/Modèle-audit-SEO.xlsx
+++ b/audit/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Documents\PROJET4\audit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA73E02-B06D-45D4-B7FE-A01CF7FD3FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353EB43A-408B-42EC-8986-DE504FBE03AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
   <si>
     <t>Catégorie</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Les partenariats sont peu pertinents et douteux</t>
   </si>
   <si>
-    <t>Aucun effet au survol sur la barre de navigation</t>
-  </si>
-  <si>
     <t>Créer une rubrique actualité</t>
   </si>
   <si>
@@ -108,15 +105,6 @@
     <t>Page non actualisée</t>
   </si>
   <si>
-    <t>Peu attractif et le visiteur hésitera avant de cliquer</t>
-  </si>
-  <si>
-    <t>Petit effet de surbrillance suffit</t>
-  </si>
-  <si>
-    <t>Il faut rendre le site le plus accessible possible</t>
-  </si>
-  <si>
     <t>La localisation est un facteur très important dans la recherche est ne doit pas être erronée</t>
   </si>
   <si>
@@ -253,6 +241,15 @@
   </si>
   <si>
     <t>Supprimer ces mots clés cachés et utiliser des méthodes "white hat"</t>
+  </si>
+  <si>
+    <t>Fichiers css mal intégrés sur le code html</t>
+  </si>
+  <si>
+    <t>Cela entraîne ici, une présentation spartiate de la page contact</t>
+  </si>
+  <si>
+    <t>Bien vérifier les extensions et la bonne prise en charge de tous les fichiers</t>
   </si>
 </sst>
 </file>
@@ -307,7 +304,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,14 +317,8 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -378,17 +369,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -426,7 +406,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -442,7 +422,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -466,35 +446,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -716,7 +693,7 @@
   <dimension ref="A1:Z1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -771,312 +748,310 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>15</v>
+      <c r="A3" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>15</v>
+      <c r="A4" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="31.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>15</v>
+      <c r="A5" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>60</v>
+      <c r="E5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>15</v>
+      <c r="A6" s="23" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="31.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:26" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:26" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="17"/>
-    </row>
-    <row r="13" spans="1:26" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="16" t="s">
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:26" ht="52.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="16"/>
-    </row>
-    <row r="16" spans="1:26" ht="41.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="B16" s="3" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="17"/>
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>61</v>
+        <v>12</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="46.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="23"/>
+        <v>23</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -2102,7 +2077,7 @@
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D13:E13"/>
@@ -2114,6 +2089,7 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F17:F18"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>